<commit_message>
Added user to seeder
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>fullName</t>
   </si>
@@ -35,9 +35,6 @@
     <t>categories_array</t>
   </si>
   <si>
-    <t>userId</t>
-  </si>
-  <si>
     <t>eventIds_array</t>
   </si>
   <si>
@@ -105,6 +102,30 @@
   </si>
   <si>
     <t>5a847edee5847831acb269ae</t>
+  </si>
+  <si>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>aa847edee5847831acb269a4</t>
+  </si>
+  <si>
+    <t>aa847edee5847831acb269a7</t>
+  </si>
+  <si>
+    <t>aa847edee5847831acb269a8</t>
+  </si>
+  <si>
+    <t>aa847edee5847831acb269a9</t>
+  </si>
+  <si>
+    <t>aa847edee5847831acb269a5</t>
+  </si>
+  <si>
+    <t>aa847edee5847831acb269a6</t>
+  </si>
+  <si>
+    <t>aa847edee5847831acb269aa</t>
   </si>
 </sst>
 </file>
@@ -459,7 +480,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,6 +488,7 @@
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="3" max="3" width="26.140625" customWidth="1"/>
     <col min="4" max="4" width="51.7109375" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -480,114 +502,136 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>